<commit_message>
adds formula to calculate values for each cell
</commit_message>
<xml_diff>
--- a/ch13/practice/multiplicationTable.xlsx
+++ b/ch13/practice/multiplicationTable.xlsx
@@ -382,30 +382,174 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="B2">
+        <f>B1 * A2</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>C1 * A2</f>
+        <v/>
+      </c>
+      <c r="D2">
+        <f>D1 * A2</f>
+        <v/>
+      </c>
+      <c r="E2">
+        <f>E1 * A2</f>
+        <v/>
+      </c>
+      <c r="F2">
+        <f>F1 * A2</f>
+        <v/>
+      </c>
+      <c r="G2">
+        <f>G1 * A2</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="B3">
+        <f>B1 * A3</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>C1 * A3</f>
+        <v/>
+      </c>
+      <c r="D3">
+        <f>D1 * A3</f>
+        <v/>
+      </c>
+      <c r="E3">
+        <f>E1 * A3</f>
+        <v/>
+      </c>
+      <c r="F3">
+        <f>F1 * A3</f>
+        <v/>
+      </c>
+      <c r="G3">
+        <f>G1 * A3</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="B4">
+        <f>B1 * A4</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>C1 * A4</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>D1 * A4</f>
+        <v/>
+      </c>
+      <c r="E4">
+        <f>E1 * A4</f>
+        <v/>
+      </c>
+      <c r="F4">
+        <f>F1 * A4</f>
+        <v/>
+      </c>
+      <c r="G4">
+        <f>G1 * A4</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="B5">
+        <f>B1 * A5</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>C1 * A5</f>
+        <v/>
+      </c>
+      <c r="D5">
+        <f>D1 * A5</f>
+        <v/>
+      </c>
+      <c r="E5">
+        <f>E1 * A5</f>
+        <v/>
+      </c>
+      <c r="F5">
+        <f>F1 * A5</f>
+        <v/>
+      </c>
+      <c r="G5">
+        <f>G1 * A5</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="B6">
+        <f>B1 * A6</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>C1 * A6</f>
+        <v/>
+      </c>
+      <c r="D6">
+        <f>D1 * A6</f>
+        <v/>
+      </c>
+      <c r="E6">
+        <f>E1 * A6</f>
+        <v/>
+      </c>
+      <c r="F6">
+        <f>F1 * A6</f>
+        <v/>
+      </c>
+      <c r="G6">
+        <f>G1 * A6</f>
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="B7">
+        <f>B1 * A7</f>
+        <v/>
+      </c>
+      <c r="C7">
+        <f>C1 * A7</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>D1 * A7</f>
+        <v/>
+      </c>
+      <c r="E7">
+        <f>E1 * A7</f>
+        <v/>
+      </c>
+      <c r="F7">
+        <f>F1 * A7</f>
+        <v/>
+      </c>
+      <c r="G7">
+        <f>G1 * A7</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>